<commit_message>
commented out stuff to get back to state of q1
</commit_message>
<xml_diff>
--- a/Project 3/p3-results.xlsx
+++ b/Project 3/p3-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quinnipiacuniversity-my.sharepoint.com/personal/bconeill_quinnipiac_edu/Documents/Documents/CSC 350-500 AI/Projects/Project 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thean\CSC.Code\CSC350\Clustering\Clustering-CSC350\Project 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{6D7F0FA9-3B6F-4247-966F-E9988896F06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6343AFF2-75D7-4204-8878-01C869DB64C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EED6365-6ED7-4D30-BE35-9B13E987D556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF08A997-3A99-4B2C-BEDC-14A11E32874A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{FF08A997-3A99-4B2C-BEDC-14A11E32874A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,6 +627,9 @@
         <f>MIN(B3:D3)</f>
         <v>0</v>
       </c>
+      <c r="H3" s="4">
+        <v>22.530999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -640,6 +643,9 @@
         <f t="shared" ref="F4:F24" si="1">MIN(B4:D4)</f>
         <v>0</v>
       </c>
+      <c r="H4" s="4">
+        <v>9.7799999999999994</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -653,6 +659,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H5" s="4">
+        <v>1.079</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -666,6 +675,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H6" s="4">
+        <v>0.505</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -679,6 +691,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H7" s="4">
+        <v>0.55400000000000005</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -692,6 +707,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H8" s="4">
+        <v>0.49199999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -705,6 +723,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H9" s="4">
+        <v>4.6669999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -718,6 +739,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H10" s="4">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -731,6 +755,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H11" s="4">
+        <v>1.417</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -744,6 +771,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H12" s="4">
+        <v>0.40799999999999997</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -757,6 +787,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H13" s="4">
+        <v>0.79700000000000004</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -770,6 +803,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H14" s="4">
+        <v>1.218</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -783,6 +819,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H15" s="4">
+        <v>0.45700000000000002</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -796,8 +835,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H16" s="4">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -809,8 +851,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H17" s="4">
+        <v>0.40899999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -822,8 +867,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H18" s="4">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -835,8 +883,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H19" s="4">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -848,8 +899,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H20" s="4">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -861,8 +915,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H21" s="4">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -874,8 +931,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H22" s="4">
+        <v>0.63100000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -887,8 +947,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H23" s="4">
+        <v>2.1469999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -899,6 +962,9 @@
       <c r="F24" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1.2430000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -907,5 +973,6 @@
     <mergeCell ref="J1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>